<commit_message>
update aerosol, atmos, toplevel for cmcc-cm2-hr4 and cmcc-cm2-vhr4 (from D.Peano)
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-hr4/cmip6_cmcc_cmcc-cm2-hr4_aerosol.xlsx
+++ b/cmip6/models/cmcc-cm2-hr4/cmip6_cmcc_cmcc-cm2-hr4_aerosol.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielepeano/Documents/ES-Doc/HR4-VHR4/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5682327-EF2B-494D-B251-FF690788BA6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23200" windowHeight="14740" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -17,12 +23,12 @@
     <sheet name="6. Optical Radiative Properties" sheetId="8" r:id="rId8"/>
     <sheet name="7. Model" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="516">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1507,13 +1513,76 @@
   </si>
   <si>
     <t>STS (supercooled ternary solution aerosol particule)</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>SCOCCIMARRO-ENRICO</t>
+  </si>
+  <si>
+    <t>Point of Contact</t>
+  </si>
+  <si>
+    <t>BELLUCCI-ALESSIO</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>PEANO-DANIELE</t>
+  </si>
+  <si>
+    <t>MACv2-SP</t>
+  </si>
+  <si>
+    <t>MACv2-SP, plume, Twomey effect</t>
+  </si>
+  <si>
+    <t>MACv2-SP is formulated in terms of nine spatial plumes associated with different major anthropogenic source regions. The shape of the plumes is fit to the Max Planck Institute Aerosol Climatology, version 2, whose present-day (2005) distribution is anchored by surface-based observations. Two types of plumes are considered: one predominantly associated with biomass burning, the other with industrial emissions. These differ in the prescription of their annual cycle and in their optical properties, thereby implicitly accounting for different contributions of absorbing aerosol to the different plumes. A Twomey effect for each plume is prescribed as a change in the host model's background cloud-droplet population density using relationships derived from satellite data. Year-to-year variations in the amplitude of the plumes over the historical period (1850–2016) are derived by scaling the plumes with associated national emission sources of SO2 and NH3. Further details in Stevens_2017</t>
+  </si>
+  <si>
+    <t>Stevens_2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nine plumes (five industrial and four biomass) appear to adequately capture the spatial distribution of the anthropogenic aerosol of MACv2; A basic premise in the development of MACv2-SP is that the shape of individual plumes is independent of the strength of the source. This assumption is reasonable as long as effects from changes in the atmospheric circulation remain small relative to uncertainty in the aerosol pattern for a given source. </t>
+  </si>
+  <si>
+    <t>plume amplitude</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5194/gmd-10-433-2017-supplement</t>
+  </si>
+  <si>
+    <t>fortran</t>
+  </si>
+  <si>
+    <t>yearly values</t>
+  </si>
+  <si>
+    <t>f09</t>
+  </si>
+  <si>
+    <t>0.9 x 1.25 degrees lat-lon</t>
+  </si>
+  <si>
+    <t>The quasi-Gaussian features are elongated to mimic asymmetric transport with prevailing winds and a possibly asymmetric distributions of sources and sinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The MACv2-SP basic idea is to associate spatial plumes of anthropogenic aerosols with emissions from source regions. The plumes are constructed by fitting to a climatology for the present-day (2005) distribution of anthropogenic aerosol optical depths in the mid-visible (550 nm) range. To capture past changes, the amplitude of these plumes will be scaled with the strength of the anthropogenic emissions within the source region. Major anthropogenic emissions are spatially compact, at least from a planetary perspective. Two plume types are considered: one that is dominated by emissions from industrial emissions, the other from biomass burning. </t>
+  </si>
+  <si>
+    <t>Optical properties are defined as a function of plume type.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Twomey effect for each plume is prescribed as a change in the host model’s background cloud-droplet population density using relationships derived from satellite data. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1709,6 +1778,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1755,7 +1832,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1787,9 +1864,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1821,6 +1916,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1996,24 +2109,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2021,7 +2134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2029,7 +2142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -2037,7 +2150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2053,37 +2166,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2091,7 +2204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>19</v>
       </c>
@@ -2099,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>21</v>
       </c>
@@ -2107,7 +2220,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -2115,13 +2228,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -2129,54 +2242,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1"/>
-    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>32</v>
       </c>
@@ -2184,70 +2299,112 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="9" t="s">
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>498</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8" t="s">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="10" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Transport,Emissions,Concentrations,Optical Radiative Properties,Model"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD145"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AI145"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>38</v>
       </c>
@@ -2255,12 +2412,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>41</v>
       </c>
@@ -2268,7 +2425,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -2279,10 +2436,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>46</v>
       </c>
@@ -2290,7 +2449,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -2301,15 +2460,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>51</v>
       </c>
@@ -2317,7 +2478,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>43</v>
       </c>
@@ -2328,15 +2489,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
-    </row>
-    <row r="18" spans="1:31" ht="24" customHeight="1">
+    <row r="16" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>56</v>
       </c>
@@ -2344,7 +2507,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="24" customHeight="1">
+    <row r="19" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -2355,13 +2518,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="24" customHeight="1">
+    <row r="20" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="24" customHeight="1">
-      <c r="B21" s="11"/>
+    <row r="21" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="AA21" s="6" t="s">
         <v>61</v>
       </c>
@@ -2378,7 +2543,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" customHeight="1">
+    <row r="23" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>66</v>
       </c>
@@ -2386,7 +2551,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" customHeight="1">
+    <row r="24" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>43</v>
       </c>
@@ -2397,10 +2562,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" customHeight="1">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="27" spans="1:31" ht="24" customHeight="1">
+    <row r="25" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>70</v>
       </c>
@@ -2408,7 +2575,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="24" customHeight="1">
+    <row r="28" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>58</v>
       </c>
@@ -2419,13 +2586,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="24" customHeight="1">
+    <row r="29" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="24" customHeight="1">
-      <c r="B30" s="11"/>
+    <row r="30" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>506</v>
+      </c>
       <c r="AA30" s="6" t="s">
         <v>74</v>
       </c>
@@ -2436,7 +2608,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="24" customHeight="1">
+    <row r="32" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>76</v>
       </c>
@@ -2444,7 +2616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>78</v>
       </c>
@@ -2455,10 +2627,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="11"/>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
+    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>81</v>
       </c>
@@ -2466,7 +2638,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>83</v>
       </c>
@@ -2477,10 +2649,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
-      <c r="B38" s="11"/>
-    </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>86</v>
       </c>
@@ -2488,12 +2662,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
+    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
+    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>89</v>
       </c>
@@ -2501,7 +2675,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
+    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>43</v>
       </c>
@@ -2512,10 +2686,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
-      <c r="B46" s="11"/>
-    </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
+    <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>93</v>
       </c>
@@ -2523,7 +2699,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="24" customHeight="1">
+    <row r="49" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>43</v>
       </c>
@@ -2534,10 +2710,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="24" customHeight="1">
+    <row r="50" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="11"/>
     </row>
-    <row r="52" spans="1:30" ht="24" customHeight="1">
+    <row r="52" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>97</v>
       </c>
@@ -2545,7 +2721,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="24" customHeight="1">
+    <row r="53" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>43</v>
       </c>
@@ -2556,15 +2732,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="24" customHeight="1">
+    <row r="54" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="24" customHeight="1">
-      <c r="B55" s="11"/>
-    </row>
-    <row r="58" spans="1:30" ht="24" customHeight="1">
+    <row r="55" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="11" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
         <v>101</v>
       </c>
@@ -2572,12 +2750,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:30" ht="24" customHeight="1">
+    <row r="59" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:30" ht="24" customHeight="1">
+    <row r="61" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>104</v>
       </c>
@@ -2585,7 +2763,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:30" ht="24" customHeight="1">
+    <row r="62" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
         <v>58</v>
       </c>
@@ -2596,8 +2774,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:30" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+    <row r="63" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>509</v>
+      </c>
       <c r="AA63" s="6" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2794,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:35" ht="24" customHeight="1">
+    <row r="65" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>111</v>
       </c>
@@ -2619,7 +2802,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="66" spans="1:35" ht="24" customHeight="1">
+    <row r="66" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>78</v>
       </c>
@@ -2630,10 +2813,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:35" ht="24" customHeight="1">
+    <row r="67" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="11"/>
     </row>
-    <row r="69" spans="1:35" ht="24" customHeight="1">
+    <row r="69" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>115</v>
       </c>
@@ -2641,7 +2824,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:35" ht="24" customHeight="1">
+    <row r="70" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
         <v>78</v>
       </c>
@@ -2652,10 +2835,10 @@
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:35" ht="24" customHeight="1">
+    <row r="71" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="11"/>
     </row>
-    <row r="73" spans="1:35" ht="24" customHeight="1">
+    <row r="73" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>119</v>
       </c>
@@ -2663,7 +2846,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:35" ht="24" customHeight="1">
+    <row r="74" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>78</v>
       </c>
@@ -2674,10 +2857,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:35" ht="24" customHeight="1">
+    <row r="75" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="11"/>
     </row>
-    <row r="77" spans="1:35" ht="24" customHeight="1">
+    <row r="77" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>123</v>
       </c>
@@ -2685,7 +2868,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="78" spans="1:35" ht="24" customHeight="1">
+    <row r="78" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="14" t="s">
         <v>58</v>
       </c>
@@ -2696,7 +2879,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="79" spans="1:35" ht="24" customHeight="1">
+    <row r="79" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="11"/>
       <c r="AA79" s="6" t="s">
         <v>127</v>
@@ -2726,7 +2909,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="24" customHeight="1">
+    <row r="82" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12" t="s">
         <v>135</v>
       </c>
@@ -2734,10 +2917,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24" customHeight="1">
+    <row r="83" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="13"/>
     </row>
-    <row r="85" spans="1:3" ht="24" customHeight="1">
+    <row r="85" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>137</v>
       </c>
@@ -2745,7 +2928,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="24" customHeight="1">
+    <row r="86" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
         <v>43</v>
       </c>
@@ -2756,15 +2939,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="24" customHeight="1">
+    <row r="87" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="24" customHeight="1">
+    <row r="88" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="11"/>
     </row>
-    <row r="90" spans="1:3" ht="24" customHeight="1">
+    <row r="90" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
         <v>141</v>
       </c>
@@ -2772,7 +2955,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="24" customHeight="1">
+    <row r="91" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
         <v>43</v>
       </c>
@@ -2783,15 +2966,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="24" customHeight="1">
+    <row r="92" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="24" customHeight="1">
+    <row r="93" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="11"/>
     </row>
-    <row r="95" spans="1:3" ht="24" customHeight="1">
+    <row r="95" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>145</v>
       </c>
@@ -2799,7 +2982,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24" customHeight="1">
+    <row r="96" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
         <v>78</v>
       </c>
@@ -2810,10 +2993,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24" customHeight="1">
+    <row r="97" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="11"/>
     </row>
-    <row r="100" spans="1:3" ht="24" customHeight="1">
+    <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
         <v>149</v>
       </c>
@@ -2821,12 +3004,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24" customHeight="1">
+    <row r="101" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="13" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
+    <row r="103" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>152</v>
       </c>
@@ -2834,7 +3017,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
+    <row r="104" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
         <v>43</v>
       </c>
@@ -2845,10 +3028,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
-    </row>
-    <row r="107" spans="1:3" ht="24" customHeight="1">
+    <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>155</v>
       </c>
@@ -2856,7 +3041,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="24" customHeight="1">
+    <row r="108" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
         <v>43</v>
       </c>
@@ -2867,10 +3052,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="24" customHeight="1">
-      <c r="B109" s="11"/>
-    </row>
-    <row r="111" spans="1:3" ht="24" customHeight="1">
+    <row r="109" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="11" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
         <v>159</v>
       </c>
@@ -2878,7 +3065,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="24" customHeight="1">
+    <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="14" t="s">
         <v>78</v>
       </c>
@@ -2889,10 +3076,10 @@
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24" customHeight="1">
+    <row r="113" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="11"/>
     </row>
-    <row r="115" spans="1:3" ht="24" customHeight="1">
+    <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
         <v>163</v>
       </c>
@@ -2900,7 +3087,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="24" customHeight="1">
+    <row r="116" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="14" t="s">
         <v>78</v>
       </c>
@@ -2911,10 +3098,10 @@
         <v>166</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="24" customHeight="1">
+    <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="11"/>
     </row>
-    <row r="119" spans="1:3" ht="24" customHeight="1">
+    <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
         <v>167</v>
       </c>
@@ -2922,7 +3109,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="24" customHeight="1">
+    <row r="120" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="14" t="s">
         <v>83</v>
       </c>
@@ -2933,10 +3120,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="24" customHeight="1">
+    <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="11"/>
     </row>
-    <row r="124" spans="1:3" ht="24" customHeight="1">
+    <row r="124" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
         <v>171</v>
       </c>
@@ -2944,12 +3131,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="24" customHeight="1">
+    <row r="125" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="13" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24" customHeight="1">
+    <row r="127" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
         <v>174</v>
       </c>
@@ -2957,7 +3144,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="24" customHeight="1">
+    <row r="128" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="14" t="s">
         <v>43</v>
       </c>
@@ -2968,15 +3155,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" customHeight="1">
+    <row r="129" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="178" customHeight="1">
+    <row r="130" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="11"/>
     </row>
-    <row r="132" spans="1:3" ht="24" customHeight="1">
+    <row r="132" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="9" t="s">
         <v>178</v>
       </c>
@@ -2984,7 +3171,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="24" customHeight="1">
+    <row r="133" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="14" t="s">
         <v>43</v>
       </c>
@@ -2995,15 +3182,15 @@
         <v>181</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="24" customHeight="1">
+    <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="24" customHeight="1">
+    <row r="135" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="11"/>
     </row>
-    <row r="137" spans="1:3" ht="24" customHeight="1">
+    <row r="137" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="9" t="s">
         <v>182</v>
       </c>
@@ -3011,7 +3198,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="24" customHeight="1">
+    <row r="138" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="14" t="s">
         <v>43</v>
       </c>
@@ -3022,15 +3209,15 @@
         <v>185</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="24" customHeight="1">
+    <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" customHeight="1">
+    <row r="140" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="11"/>
     </row>
-    <row r="142" spans="1:3" ht="24" customHeight="1">
+    <row r="142" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
         <v>186</v>
       </c>
@@ -3038,7 +3225,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="24" customHeight="1">
+    <row r="143" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="14" t="s">
         <v>43</v>
       </c>
@@ -3049,54 +3236,33 @@
         <v>189</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="24" customHeight="1">
+    <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="24" customHeight="1">
+    <row r="145" spans="2:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="13">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA21:AE21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AA30:AC30</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34 B117 B113 B97 B75 B71 B67" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38 B121" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>AA63:AD63</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>AA79:AI79</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B113">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B117">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B121">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3104,20 +3270,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>190</v>
       </c>
@@ -3125,12 +3293,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>193</v>
       </c>
@@ -3138,7 +3306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -3149,10 +3317,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>196</v>
       </c>
@@ -3160,7 +3330,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -3171,15 +3341,15 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
     </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>199</v>
       </c>
@@ -3187,7 +3357,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>83</v>
       </c>
@@ -3198,10 +3368,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
-      <c r="B15" s="11"/>
-    </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>203</v>
       </c>
@@ -3209,12 +3381,12 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
+    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>206</v>
       </c>
@@ -3222,7 +3394,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>43</v>
       </c>
@@ -3233,10 +3405,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
-      <c r="B23" s="11"/>
-    </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>208</v>
       </c>
@@ -3244,7 +3418,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>43</v>
       </c>
@@ -3255,10 +3429,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
-    </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1">
+    <row r="27" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="11" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>211</v>
       </c>
@@ -3266,7 +3442,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="24" customHeight="1">
+    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>78</v>
       </c>
@@ -3277,10 +3453,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11"/>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>213</v>
       </c>
@@ -3288,7 +3464,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>78</v>
       </c>
@@ -3299,10 +3475,10 @@
         <v>214</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="11"/>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>215</v>
       </c>
@@ -3310,7 +3486,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>83</v>
       </c>
@@ -3321,22 +3497,16 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B39" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B35" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3344,20 +3514,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="24" customHeight="1">
+    <row r="1" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>218</v>
       </c>
@@ -3365,12 +3537,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="24" customHeight="1">
+    <row r="2" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="24" customHeight="1">
+    <row r="4" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>221</v>
       </c>
@@ -3378,7 +3550,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="24" customHeight="1">
+    <row r="5" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -3389,10 +3561,10 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="24" customHeight="1">
+    <row r="6" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:31" ht="24" customHeight="1">
+    <row r="8" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>224</v>
       </c>
@@ -3400,7 +3572,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="24" customHeight="1">
+    <row r="9" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -3411,15 +3583,17 @@
         <v>226</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="24" customHeight="1">
+    <row r="10" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:31" ht="24" customHeight="1">
+    <row r="11" spans="1:31" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>227</v>
       </c>
@@ -3427,7 +3601,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="24" customHeight="1">
+    <row r="14" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>58</v>
       </c>
@@ -3438,7 +3612,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="24" customHeight="1">
+    <row r="15" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
       <c r="AA15" s="6" t="s">
         <v>231</v>
@@ -3456,7 +3630,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="24" customHeight="1">
+    <row r="17" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>236</v>
       </c>
@@ -3464,7 +3638,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="24" customHeight="1">
+    <row r="18" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>58</v>
       </c>
@@ -3475,12 +3649,12 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="24" customHeight="1">
+    <row r="19" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="24" customHeight="1">
+    <row r="20" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="11"/>
       <c r="AA20" s="6" t="s">
         <v>231</v>
@@ -3498,7 +3672,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="24" customHeight="1">
+    <row r="22" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>243</v>
       </c>
@@ -3506,7 +3680,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="24" customHeight="1">
+    <row r="23" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -3517,12 +3691,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="24" customHeight="1">
+    <row r="24" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="24" customHeight="1">
+    <row r="25" spans="1:31" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11"/>
       <c r="AA25" s="6" t="s">
         <v>231</v>
@@ -3538,14 +3712,11 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B20" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>AA15:AE15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
-      <formula1>AA20:AE20</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>AA25:AD25</formula1>
     </dataValidation>
   </dataValidations>
@@ -3554,20 +3725,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="24" customHeight="1">
+    <row r="1" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>249</v>
       </c>
@@ -3575,12 +3748,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="24" customHeight="1">
+    <row r="2" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="24" customHeight="1">
+    <row r="4" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>252</v>
       </c>
@@ -3588,7 +3761,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="24" customHeight="1">
+    <row r="5" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -3599,10 +3772,10 @@
         <v>254</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="24" customHeight="1">
+    <row r="6" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:33" ht="24" customHeight="1">
+    <row r="8" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>255</v>
       </c>
@@ -3610,7 +3783,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="24" customHeight="1">
+    <row r="9" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -3621,15 +3794,17 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="24" customHeight="1">
+    <row r="10" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:33" ht="24" customHeight="1">
+    <row r="11" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>258</v>
       </c>
@@ -3637,7 +3812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="24" customHeight="1">
+    <row r="14" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>58</v>
       </c>
@@ -3648,13 +3823,15 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="24" customHeight="1">
+    <row r="15" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="24" customHeight="1">
-      <c r="B16" s="11"/>
+    <row r="16" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>263</v>
+      </c>
       <c r="AA16" s="6" t="s">
         <v>261</v>
       </c>
@@ -3677,7 +3854,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
+    <row r="18" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>267</v>
       </c>
@@ -3685,7 +3862,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
+    <row r="19" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -3696,12 +3873,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
+    <row r="20" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="AA21" s="6" t="s">
         <v>271</v>
@@ -3731,7 +3908,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
+    <row r="23" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>279</v>
       </c>
@@ -3739,7 +3916,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>58</v>
       </c>
@@ -3750,7 +3927,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1">
+    <row r="25" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11"/>
       <c r="AA25" s="6" t="s">
         <v>283</v>
@@ -3768,7 +3945,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="27" spans="1:35" ht="24" customHeight="1">
+    <row r="27" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>288</v>
       </c>
@@ -3776,7 +3953,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
+    <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>43</v>
       </c>
@@ -3787,15 +3964,15 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1">
+    <row r="29" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
+    <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11"/>
     </row>
-    <row r="32" spans="1:35" ht="24" customHeight="1">
+    <row r="32" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>292</v>
       </c>
@@ -3803,7 +3980,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>43</v>
       </c>
@@ -3814,15 +3991,15 @@
         <v>295</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="11"/>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>296</v>
       </c>
@@ -3830,7 +4007,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>43</v>
       </c>
@@ -3841,15 +4018,15 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
+    <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="11"/>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
+    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>300</v>
       </c>
@@ -3857,7 +4034,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>43</v>
       </c>
@@ -3868,15 +4045,15 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
+    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
+    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="11"/>
     </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1">
+    <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>304</v>
       </c>
@@ -3884,7 +4061,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
+    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>43</v>
       </c>
@@ -3895,18 +4072,18 @@
         <v>307</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="24" customHeight="1">
+    <row r="49" spans="2:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>AA16:AG16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>AA21:AI21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>AA25:AE25</formula1>
     </dataValidation>
   </dataValidations>
@@ -3915,20 +4092,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>308</v>
       </c>
@@ -3936,12 +4113,12 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>311</v>
       </c>
@@ -3949,7 +4126,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -3960,10 +4137,10 @@
         <v>313</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>314</v>
       </c>
@@ -3971,7 +4148,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -3982,15 +4159,15 @@
         <v>316</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
     </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>317</v>
       </c>
@@ -3998,7 +4175,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>43</v>
       </c>
@@ -4009,15 +4186,15 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="24" customHeight="1">
+    <row r="16" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>321</v>
       </c>
@@ -4025,7 +4202,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>43</v>
       </c>
@@ -4036,15 +4213,15 @@
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
+    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
+    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>325</v>
       </c>
@@ -4052,7 +4229,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>43</v>
       </c>
@@ -4063,15 +4240,15 @@
         <v>328</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11"/>
     </row>
-    <row r="28" spans="1:3" ht="24" customHeight="1">
+    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>329</v>
       </c>
@@ -4079,7 +4256,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1">
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>43</v>
       </c>
@@ -4090,12 +4267,12 @@
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="24" customHeight="1">
+    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11"/>
     </row>
   </sheetData>
@@ -4104,20 +4281,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>333</v>
       </c>
@@ -4125,12 +4304,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>336</v>
       </c>
@@ -4138,7 +4317,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -4149,10 +4328,10 @@
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>339</v>
       </c>
@@ -4160,7 +4339,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -4171,15 +4350,17 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>342</v>
       </c>
@@ -4187,12 +4368,12 @@
         <v>343</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
+    <row r="17" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>345</v>
       </c>
@@ -4200,7 +4381,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24" customHeight="1">
+    <row r="18" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>347</v>
       </c>
@@ -4211,10 +4392,10 @@
         <v>349</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="11"/>
     </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1">
+    <row r="21" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>350</v>
       </c>
@@ -4222,7 +4403,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>347</v>
       </c>
@@ -4233,10 +4414,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
     </row>
-    <row r="25" spans="1:3" ht="24" customHeight="1">
+    <row r="25" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>354</v>
       </c>
@@ -4244,7 +4425,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="24" customHeight="1">
+    <row r="26" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>347</v>
       </c>
@@ -4255,10 +4436,10 @@
         <v>357</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="24" customHeight="1">
+    <row r="27" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="11"/>
     </row>
-    <row r="30" spans="1:3" ht="24" customHeight="1">
+    <row r="30" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>358</v>
       </c>
@@ -4266,10 +4447,10 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13"/>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>360</v>
       </c>
@@ -4277,7 +4458,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="24" customHeight="1">
+    <row r="34" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>83</v>
       </c>
@@ -4288,10 +4469,12 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
-      <c r="B35" s="11"/>
-    </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>364</v>
       </c>
@@ -4299,7 +4482,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="24" customHeight="1">
+    <row r="38" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>83</v>
       </c>
@@ -4310,10 +4493,10 @@
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="11"/>
     </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>368</v>
       </c>
@@ -4321,7 +4504,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="24" customHeight="1">
+    <row r="42" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>43</v>
       </c>
@@ -4332,10 +4515,10 @@
         <v>371</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="11"/>
     </row>
-    <row r="46" spans="1:3" ht="24" customHeight="1">
+    <row r="46" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>372</v>
       </c>
@@ -4343,12 +4526,12 @@
         <v>373</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="24" customHeight="1">
+    <row r="47" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="24" customHeight="1">
+    <row r="49" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>375</v>
       </c>
@@ -4356,7 +4539,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24" customHeight="1">
+    <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>83</v>
       </c>
@@ -4367,10 +4550,10 @@
         <v>378</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="24" customHeight="1">
+    <row r="51" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="11"/>
     </row>
-    <row r="53" spans="1:3" ht="24" customHeight="1">
+    <row r="53" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>379</v>
       </c>
@@ -4378,7 +4561,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="24" customHeight="1">
+    <row r="54" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>83</v>
       </c>
@@ -4389,10 +4572,10 @@
         <v>382</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="24" customHeight="1">
+    <row r="55" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="11"/>
     </row>
-    <row r="57" spans="1:3" ht="24" customHeight="1">
+    <row r="57" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>383</v>
       </c>
@@ -4400,7 +4583,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="24" customHeight="1">
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
         <v>83</v>
       </c>
@@ -4411,10 +4594,10 @@
         <v>386</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="24" customHeight="1">
+    <row r="59" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="11"/>
     </row>
-    <row r="62" spans="1:3" ht="24" customHeight="1">
+    <row r="62" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
         <v>387</v>
       </c>
@@ -4422,12 +4605,12 @@
         <v>388</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="24" customHeight="1">
+    <row r="63" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="13" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="24" customHeight="1">
+    <row r="65" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>390</v>
       </c>
@@ -4435,7 +4618,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="24" customHeight="1">
+    <row r="66" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="14" t="s">
         <v>43</v>
       </c>
@@ -4446,15 +4629,15 @@
         <v>392</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="24" customHeight="1">
+    <row r="67" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="178" customHeight="1">
+    <row r="68" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="11"/>
     </row>
-    <row r="70" spans="1:3" ht="24" customHeight="1">
+    <row r="70" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>393</v>
       </c>
@@ -4462,7 +4645,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="24" customHeight="1">
+    <row r="71" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="14" t="s">
         <v>78</v>
       </c>
@@ -4473,10 +4656,10 @@
         <v>396</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="24" customHeight="1">
+    <row r="72" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="11"/>
     </row>
-    <row r="74" spans="1:3" ht="24" customHeight="1">
+    <row r="74" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>397</v>
       </c>
@@ -4484,7 +4667,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="24" customHeight="1">
+    <row r="75" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="14" t="s">
         <v>78</v>
       </c>
@@ -4495,10 +4678,10 @@
         <v>400</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="24" customHeight="1">
+    <row r="76" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="11"/>
     </row>
-    <row r="79" spans="1:3" ht="24" customHeight="1">
+    <row r="79" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
         <v>401</v>
       </c>
@@ -4506,12 +4689,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="24" customHeight="1">
+    <row r="80" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="13" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="24" customHeight="1">
+    <row r="82" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>404</v>
       </c>
@@ -4519,7 +4702,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24" customHeight="1">
+    <row r="83" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>43</v>
       </c>
@@ -4530,15 +4713,17 @@
         <v>406</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="24" customHeight="1">
+    <row r="84" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="178" customHeight="1">
-      <c r="B85" s="11"/>
-    </row>
-    <row r="87" spans="1:3" ht="24" customHeight="1">
+    <row r="85" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
         <v>407</v>
       </c>
@@ -4546,7 +4731,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="24" customHeight="1">
+    <row r="88" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
         <v>83</v>
       </c>
@@ -4557,10 +4742,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
-    </row>
-    <row r="91" spans="1:3" ht="24" customHeight="1">
+    <row r="89" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
         <v>411</v>
       </c>
@@ -4568,7 +4755,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="24" customHeight="1">
+    <row r="92" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
         <v>78</v>
       </c>
@@ -4579,10 +4766,10 @@
         <v>414</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="24" customHeight="1">
+    <row r="93" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="11"/>
     </row>
-    <row r="95" spans="1:3" ht="24" customHeight="1">
+    <row r="95" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>415</v>
       </c>
@@ -4590,7 +4777,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24" customHeight="1">
+    <row r="96" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
         <v>83</v>
       </c>
@@ -4601,10 +4788,10 @@
         <v>418</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24" customHeight="1">
+    <row r="97" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="11"/>
     </row>
-    <row r="99" spans="1:3" ht="24" customHeight="1">
+    <row r="99" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
         <v>419</v>
       </c>
@@ -4612,7 +4799,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="24" customHeight="1">
+    <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="14" t="s">
         <v>83</v>
       </c>
@@ -4623,10 +4810,10 @@
         <v>422</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24" customHeight="1">
+    <row r="101" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="11"/>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
+    <row r="103" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>423</v>
       </c>
@@ -4634,7 +4821,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
+    <row r="104" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="14" t="s">
         <v>78</v>
       </c>
@@ -4645,57 +4832,19 @@
         <v>424</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
+    <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B27 B23" xr:uid="{00000000-0002-0000-0700-000000000000}">
+      <formula1>-1000000</formula1>
+      <formula2>1000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B27">
-      <formula1>-1000000.0</formula1>
-      <formula2>1000000.0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35 B101 B97 B89 B59 B55 B51 B39" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B93">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B97">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B101">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B105">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72 B105 B93 B76" xr:uid="{00000000-0002-0000-0700-000008000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -4704,20 +4853,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AN36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="24" customHeight="1">
+    <row r="1" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>425</v>
       </c>
@@ -4725,12 +4876,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="24" customHeight="1">
+    <row r="2" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="24" customHeight="1">
+    <row r="4" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>427</v>
       </c>
@@ -4738,7 +4889,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="24" customHeight="1">
+    <row r="5" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -4749,10 +4900,12 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:39" ht="24" customHeight="1">
+    <row r="6" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>430</v>
       </c>
@@ -4760,7 +4913,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="24" customHeight="1">
+    <row r="9" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>43</v>
       </c>
@@ -4771,15 +4924,17 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="24" customHeight="1">
+    <row r="10" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:39" ht="24" customHeight="1">
+    <row r="11" spans="1:39" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>433</v>
       </c>
@@ -4787,7 +4942,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="24" customHeight="1">
+    <row r="14" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>58</v>
       </c>
@@ -4798,12 +4953,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="24" customHeight="1">
+    <row r="15" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="24" customHeight="1">
+    <row r="16" spans="1:39" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
       <c r="AA16" s="6" t="s">
         <v>437</v>
@@ -4845,7 +5000,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="24" customHeight="1">
+    <row r="18" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>450</v>
       </c>
@@ -4853,7 +5008,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="24" customHeight="1">
+    <row r="19" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>58</v>
       </c>
@@ -4864,12 +5019,12 @@
         <v>453</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="24" customHeight="1">
+    <row r="20" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="24" customHeight="1">
+    <row r="21" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
       <c r="AA21" s="6" t="s">
         <v>454</v>
@@ -4896,7 +5051,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="24" customHeight="1">
+    <row r="23" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>460</v>
       </c>
@@ -4904,7 +5059,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="24" spans="1:35" ht="24" customHeight="1">
+    <row r="24" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>58</v>
       </c>
@@ -4915,12 +5070,12 @@
         <v>463</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="24" customHeight="1">
+    <row r="25" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:35" ht="24" customHeight="1">
+    <row r="26" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="11"/>
       <c r="AA26" s="6" t="s">
         <v>464</v>
@@ -4950,7 +5105,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:35" ht="24" customHeight="1">
+    <row r="28" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>472</v>
       </c>
@@ -4958,7 +5113,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="24" customHeight="1">
+    <row r="29" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>58</v>
       </c>
@@ -4969,12 +5124,12 @@
         <v>475</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="24" customHeight="1">
+    <row r="30" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:35" ht="24" customHeight="1">
+    <row r="31" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="11"/>
       <c r="AA31" s="6" t="s">
         <v>476</v>
@@ -4989,7 +5144,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:40" ht="24" customHeight="1">
+    <row r="33" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>479</v>
       </c>
@@ -4997,7 +5152,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="34" spans="1:40" ht="24" customHeight="1">
+    <row r="34" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>58</v>
       </c>
@@ -5008,12 +5163,12 @@
         <v>482</v>
       </c>
     </row>
-    <row r="35" spans="1:40" ht="24" customHeight="1">
+    <row r="35" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="24" customHeight="1">
+    <row r="36" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="11"/>
       <c r="AA36" s="6" t="s">
         <v>483</v>
@@ -5060,19 +5215,19 @@
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>AA16:AM16</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>AA21:AH21</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>AA26:AI26</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>AA31:AD31</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36" xr:uid="{00000000-0002-0000-0800-000004000000}">
       <formula1>AA36:AN36</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>